<commit_message>
Initial commit of STM32 firmware.
</commit_message>
<xml_diff>
--- a/kicad/rpi_sensor_hat.xlsx
+++ b/kicad/rpi_sensor_hat.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eoberholzer\Documents\Projects\rpi_sensor_hat\kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{10591D71-EFDC-424F-83C3-958583E0EA57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FBAEB-81BD-46A2-9A94-CE2F6BE06FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rpi_sensor_hat" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">rpi_sensor_hat!$A$1:$H$23</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -247,16 +250,25 @@
     <t>R5, R6, R15, R18, R19, R20, R21, R25, R26, R27</t>
   </si>
   <si>
-    <t>R7, R8, R9, R10, R11, R12, R13, R14, R22, R23, R24, R28</t>
-  </si>
-  <si>
     <t>Tot</t>
+  </si>
+  <si>
+    <t>R8, R13, R22</t>
+  </si>
+  <si>
+    <t>R7, R9, R10, R11, R12, R14, R23, R24, R28</t>
+  </si>
+  <si>
+    <t>R16, R17</t>
+  </si>
+  <si>
+    <t>DNP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1090,11 +1102,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1170,7 +1182,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C21" si="0">B3*5</f>
+        <f t="shared" ref="C3:C23" si="0">B3*5</f>
         <v>5</v>
       </c>
       <c r="D3" t="s">
@@ -1515,23 +1527,23 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" t="s">
-        <v>52</v>
       </c>
       <c r="H16" t="s">
         <v>45</v>
@@ -1542,23 +1554,23 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" t="s">
         <v>45</v>
@@ -1569,26 +1581,26 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1596,26 +1608,26 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="G19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H19" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,19 +1642,19 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1657,22 +1669,77 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>65</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>68</v>
       </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
         <v>66</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>